<commit_message>
created tempoarary pages for confinanced projects
</commit_message>
<xml_diff>
--- a/FieldMapping/partner agency tab mapping.xlsx
+++ b/FieldMapping/partner agency tab mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Web Field</t>
   </si>
@@ -32,63 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">Original Agreement – Partner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contribution Commited</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Original Ammendment/Ammendment – Contribtions Tab - </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">$US Equiv.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (Applies both to Trust Funds and PSCs</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Sum of </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">$US Equiv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> of from all Original Agreements and Ammendments from Partner for boith Trust Funds and PSC</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -98,11 +41,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -124,12 +68,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,18 +148,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>15480</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>93240</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Image 1" descr=""/>
+        <xdr:cNvPr id="0" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -229,8 +168,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1125000"/>
-          <a:ext cx="18445680" cy="8252280"/>
+          <a:off x="0" y="9740880"/>
+          <a:ext cx="12675600" cy="5650920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -246,18 +185,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>93600</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>113040</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>207720</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Image 2" descr=""/>
+        <xdr:cNvPr id="1" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -266,45 +205,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="9740880"/>
-          <a:ext cx="12834000" cy="5651280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>354960</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 3" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="15593040"/>
-          <a:ext cx="14721120" cy="3623760"/>
+          <a:off x="0" y="1136520"/>
+          <a:ext cx="18390600" cy="8490960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,18 +226,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:3"/>
+  <dimension ref="1:2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="72.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="71.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,17 +257,7 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="36.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C2" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>